<commit_message>
edited requirements doc a little
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -161,9 +161,6 @@
     <t>For the first round, each player should ante 1 at a time from left to right</t>
   </si>
   <si>
-    <t>Mainwin::on_ante_click()</t>
-  </si>
-  <si>
     <t>The ante shall be set to $1 at the beginning of the game</t>
   </si>
   <si>
@@ -294,6 +291,9 @@
   </si>
   <si>
     <t>Stack::add_chips()</t>
+  </si>
+  <si>
+    <t>Mainwin::on_ante_click()/Player::move_j()</t>
   </si>
 </sst>
 </file>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1056,7 +1056,7 @@
         <v>33</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1119,7 +1119,7 @@
         <v>33</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1133,14 +1133,14 @@
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1154,14 +1154,14 @@
         <v>29</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1175,14 +1175,14 @@
         <v>29</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1196,7 +1196,7 @@
         <v>29</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="3" t="s">
@@ -1215,11 +1215,11 @@
         <v>21</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G27" s="4"/>
     </row>
@@ -1234,11 +1234,11 @@
         <v>21</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G28" s="4"/>
     </row>
@@ -1253,14 +1253,14 @@
         <v>21</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1274,14 +1274,14 @@
         <v>21</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1295,14 +1295,14 @@
         <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1316,14 +1316,14 @@
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1337,14 +1337,14 @@
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1358,14 +1358,14 @@
         <v>9</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1379,14 +1379,14 @@
         <v>9</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1400,14 +1400,14 @@
         <v>21</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1421,14 +1421,14 @@
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1442,14 +1442,14 @@
         <v>21</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1463,14 +1463,14 @@
         <v>21</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1484,14 +1484,14 @@
         <v>29</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1505,14 +1505,14 @@
         <v>29</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1526,14 +1526,14 @@
         <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1547,14 +1547,14 @@
         <v>9</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1568,14 +1568,14 @@
         <v>9</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1589,14 +1589,14 @@
         <v>9</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1610,14 +1610,14 @@
         <v>9</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1631,14 +1631,14 @@
         <v>9</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1652,14 +1652,14 @@
         <v>9</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1673,14 +1673,14 @@
         <v>9</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1694,14 +1694,14 @@
         <v>9</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1715,14 +1715,14 @@
         <v>9</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="3" t="s">
         <v>33</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1736,14 +1736,14 @@
         <v>9</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1757,13 +1757,13 @@
         <v>9</v>
       </c>
       <c r="D53" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G53" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated test cases some
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -119,9 +119,6 @@
     <t>All decisions about winning, losing, and game play are made by the dealer application</t>
   </si>
   <si>
-    <t>Most of the error checking should be done in th dealer application. The player applicaiton should contain very limited error checking</t>
-  </si>
-  <si>
     <t>The system shall generate a deck of cards that consists of 52 cards</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>Deck::Deck</t>
   </si>
   <si>
-    <t>Each card shall be assigned a suit (hearts, clubs, spades, or diamonds) and either a numerical value from 2 to 10 or a face value (J,Q,K,A)</t>
-  </si>
-  <si>
     <t>Card::_suit/_num</t>
   </si>
   <si>
@@ -294,6 +288,12 @@
   </si>
   <si>
     <t>Mainwin::on_ante_click()/Player::move_j()</t>
+  </si>
+  <si>
+    <t>Most of the error checking should be done in the dealer application. The player applicaiton should contain very limited error checking</t>
+  </si>
+  <si>
+    <t>Each card shall be assigned a suit (hearts, clubs, spades, or diamonds) and either a numerical value from 1 to 13 or a face value (J,Q,K,A)</t>
   </si>
 </sst>
 </file>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -948,7 +948,7 @@
         <v>29</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="3" t="s">
@@ -967,14 +967,14 @@
         <v>9</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="14" x14ac:dyDescent="0.3">
@@ -988,14 +988,14 @@
         <v>9</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1009,7 +1009,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="3" t="s">
@@ -1028,14 +1028,14 @@
         <v>9</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1049,14 +1049,14 @@
         <v>21</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1070,14 +1070,14 @@
         <v>29</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1091,14 +1091,14 @@
         <v>29</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1112,14 +1112,14 @@
         <v>21</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1133,14 +1133,14 @@
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1154,14 +1154,14 @@
         <v>29</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1175,14 +1175,14 @@
         <v>29</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1196,11 +1196,11 @@
         <v>29</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G26" s="4"/>
     </row>
@@ -1215,11 +1215,11 @@
         <v>21</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G27" s="4"/>
     </row>
@@ -1234,11 +1234,11 @@
         <v>21</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G28" s="4"/>
     </row>
@@ -1253,14 +1253,14 @@
         <v>21</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1274,14 +1274,14 @@
         <v>21</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1295,14 +1295,14 @@
         <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1316,14 +1316,14 @@
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1337,14 +1337,14 @@
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1358,14 +1358,14 @@
         <v>9</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1379,14 +1379,14 @@
         <v>9</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1400,14 +1400,14 @@
         <v>21</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1421,14 +1421,14 @@
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1442,14 +1442,14 @@
         <v>21</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1463,14 +1463,14 @@
         <v>21</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1484,14 +1484,14 @@
         <v>29</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1505,14 +1505,14 @@
         <v>29</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1526,14 +1526,14 @@
         <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1547,14 +1547,14 @@
         <v>9</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1568,14 +1568,14 @@
         <v>9</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1589,14 +1589,14 @@
         <v>9</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1610,14 +1610,14 @@
         <v>9</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1631,14 +1631,14 @@
         <v>9</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1652,14 +1652,14 @@
         <v>9</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1673,14 +1673,14 @@
         <v>9</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1694,14 +1694,14 @@
         <v>9</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1715,14 +1715,14 @@
         <v>9</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1736,34 +1736,35 @@
         <v>9</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
         <v>52</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>87</v>
+      <c r="B53" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated requirements and test cases further
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="88">
   <si>
     <t>REQ ID</t>
   </si>
@@ -182,9 +182,6 @@
     <t>The system shall allow players to look at their own 5 cards, but not any others</t>
   </si>
   <si>
-    <t>After each player recieves their cards, a "betting round" should begin where they should choose to either check, bet, raise call, or fold</t>
-  </si>
-  <si>
     <t>Player::move_j()</t>
   </si>
   <si>
@@ -194,27 +191,9 @@
     <t>The system will define "check" as a player retaining their current hand and making no bet</t>
   </si>
   <si>
-    <t>The system will define "bet" as the first wager set at the table during the current round</t>
-  </si>
-  <si>
-    <t>The system will define "raise" as betting over the current bet amount. Every other player must match this new amount if they want to continue</t>
-  </si>
-  <si>
-    <t>The system will define "call" as matching the current bet amount</t>
-  </si>
-  <si>
     <t>The system will define "fold" as discarding all cards and forfeiting the game</t>
   </si>
   <si>
-    <t>After the betting round completes, players shall be given the option to exhange 1-4 of their cards for new cards in the deck or stand pat</t>
-  </si>
-  <si>
-    <t>The system will define "stand pat" as exchanging 0 cards and keeping the original hand</t>
-  </si>
-  <si>
-    <t>After all players have had the chance to exchange cards, another betting round is played</t>
-  </si>
-  <si>
     <t>Round::determine_round()</t>
   </si>
   <si>
@@ -294,6 +273,21 @@
   </si>
   <si>
     <t>Each card shall be assigned a suit (hearts, clubs, spades, or diamonds) and either a numerical value from 1 to 13 or a face value (J,Q,K,A)</t>
+  </si>
+  <si>
+    <t>After each player recieves their cards, a "betting round" should begin where they should choose to either fold, check, or bet</t>
+  </si>
+  <si>
+    <t>The system will define "stand" as exchanging 0 cards and keeping the original hand</t>
+  </si>
+  <si>
+    <t>The system will define "bet" as a wager set at the table during the current round</t>
+  </si>
+  <si>
+    <t>After the betting round completes, players shall be given the option to exhange 1-4 of their cards for new cards in the deck or stand</t>
+  </si>
+  <si>
+    <t>After all players have had the chance to exchange cards or stand, another betting round is played</t>
   </si>
 </sst>
 </file>
@@ -660,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -948,7 +942,7 @@
         <v>29</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="3" t="s">
@@ -988,7 +982,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="3" t="s">
@@ -1056,7 +1050,7 @@
         <v>32</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1119,7 +1113,7 @@
         <v>32</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1253,14 +1247,14 @@
         <v>21</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1274,14 +1268,14 @@
         <v>21</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1295,14 +1289,14 @@
         <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="3" t="s">
         <v>50</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1316,14 +1310,14 @@
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="3" t="s">
         <v>50</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1337,14 +1331,14 @@
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="3" t="s">
         <v>50</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1355,17 +1349,17 @@
         <v>20</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="3" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1379,14 +1373,14 @@
         <v>9</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="3" t="s">
         <v>50</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1400,14 +1394,14 @@
         <v>21</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G36" s="5" t="s">
-        <v>53</v>
+      <c r="G36" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1418,17 +1412,17 @@
         <v>20</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>53</v>
+        <v>32</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1439,17 +1433,17 @@
         <v>20</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1460,17 +1454,17 @@
         <v>20</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="3" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1481,17 +1475,17 @@
         <v>20</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>67</v>
+      <c r="G40" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1502,17 +1496,17 @@
         <v>20</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>67</v>
+        <v>32</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1526,14 +1520,14 @@
         <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1547,14 +1541,14 @@
         <v>9</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1568,14 +1562,14 @@
         <v>9</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1589,14 +1583,14 @@
         <v>9</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1610,14 +1604,14 @@
         <v>9</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1631,14 +1625,14 @@
         <v>9</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1652,14 +1646,14 @@
         <v>9</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1673,14 +1667,14 @@
         <v>9</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="14" x14ac:dyDescent="0.3">
@@ -1694,78 +1688,54 @@
         <v>9</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="14" x14ac:dyDescent="0.3">
-      <c r="A51" s="3">
+      <c r="A51" s="7">
         <v>50</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E51" s="4"/>
-      <c r="F51" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>72</v>
+      <c r="B51" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="14" x14ac:dyDescent="0.3">
-      <c r="A52" s="3">
-        <v>51</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>81</v>
-      </c>
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
       <c r="E52" s="4"/>
-      <c r="F52" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
     </row>
     <row r="53" spans="1:7" ht="14" x14ac:dyDescent="0.3">
-      <c r="A53" s="7">
-        <v>52</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>84</v>
-      </c>
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
       <c r="E53" s="7"/>
-      <c r="F53" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>85</v>
-      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>